<commit_message>
Result figures and the script which made them
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conall De Paor\Desktop\Supaero\Research Project\Sizing-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C632EBB4-8563-4504-952F-58708CC9D548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBB20AB-6901-43FF-9324-F1F4F52DD82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{A8CC2F8B-8671-446E-BE64-E520A416B0FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A8CC2F8B-8671-446E-BE64-E520A416B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Swiss Cheese DB" sheetId="2" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t>Lander names</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Propellent</t>
   </si>
   <si>
-    <t>Inert mass</t>
-  </si>
-  <si>
     <t>Descent Thrust (N)</t>
   </si>
   <si>
@@ -397,15 +394,6 @@
     <t>SAIC Lunar Lander 0503-CE&amp;R-8 (Desc-Asc)</t>
   </si>
   <si>
-    <t>Total Mass</t>
-  </si>
-  <si>
-    <t>Dry mass</t>
-  </si>
-  <si>
-    <t>Propellant</t>
-  </si>
-  <si>
     <t>propratio</t>
   </si>
   <si>
@@ -530,6 +518,9 @@
   </si>
   <si>
     <t>power cons</t>
+  </si>
+  <si>
+    <t>inert mass</t>
   </si>
 </sst>
 </file>
@@ -537,7 +528,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -561,7 +552,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -811,10 +808,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -823,15 +820,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,7 +1177,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
@@ -1188,54 +1186,54 @@
         <v>4</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8">
         <v>15103</v>
@@ -1288,7 +1286,7 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8">
         <v>15065</v>
@@ -1341,7 +1339,7 @@
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8">
         <v>14916</v>
@@ -1394,7 +1392,7 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8">
         <v>14916</v>
@@ -1447,7 +1445,7 @@
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8">
         <v>16447</v>
@@ -1512,7 +1510,7 @@
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="8">
         <v>16447</v>
@@ -1577,7 +1575,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8">
         <v>16447</v>
@@ -1642,7 +1640,7 @@
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8">
         <v>60075</v>
@@ -1693,7 +1691,7 @@
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8">
         <v>48218</v>
@@ -1744,7 +1742,7 @@
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="8">
         <v>47600</v>
@@ -1781,7 +1779,7 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8">
         <v>93037</v>
@@ -1830,7 +1828,7 @@
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8">
         <v>93038</v>
@@ -1887,7 +1885,7 @@
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="8">
         <v>33749</v>
@@ -1924,7 +1922,7 @@
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8">
         <v>33684</v>
@@ -1961,7 +1959,7 @@
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8">
         <v>5038.6000000000004</v>
@@ -2008,7 +2006,7 @@
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="8">
         <v>54597</v>
@@ -2043,10 +2041,10 @@
         <v>1792</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P19" s="8">
         <v>36272</v>
@@ -2070,7 +2068,7 @@
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="8">
         <v>27021</v>
@@ -2101,7 +2099,7 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="8">
         <v>44821</v>
@@ -2142,7 +2140,7 @@
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="8">
         <v>52183</v>
@@ -2186,7 +2184,7 @@
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="8">
         <v>45862</v>
@@ -2248,7 +2246,7 @@
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="8">
         <v>81911</v>
@@ -2310,47 +2308,47 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F7DD18-26CD-4057-849D-39AE03A1CE0B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -2377,72 +2375,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="8">
         <v>15103</v>
@@ -2511,7 +2509,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="8">
         <v>15065</v>
@@ -2579,7 +2577,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>14916</v>
@@ -2647,7 +2645,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="8">
         <v>14916</v>
@@ -2715,7 +2713,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="8">
         <v>16447</v>
@@ -2780,7 +2778,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="8">
         <v>16447</v>
@@ -2845,7 +2843,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="8">
         <v>16447</v>
@@ -2910,7 +2908,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8">
         <v>93038</v>
@@ -2951,7 +2949,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B10" s="8">
         <v>48218</v>
@@ -2995,7 +2993,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B11" s="8">
         <v>5038.6000000000004</v>
@@ -3039,7 +3037,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B12" s="8">
         <v>45862</v>
@@ -3101,7 +3099,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B13" s="8">
         <v>81911</v>
@@ -3169,10 +3167,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80C5C0-5165-4D8F-8D34-D728F416EF6B}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,13 +3179,13 @@
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
     <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -3199,57 +3197,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>5750</v>
       </c>
       <c r="C2">
-        <v>2400</v>
+        <v>1880</v>
       </c>
       <c r="D2">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E2">
         <v>3350</v>
@@ -3266,7 +3264,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>5700</v>
@@ -3292,7 +3290,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>3780</v>
@@ -3300,7 +3298,7 @@
       <c r="C4">
         <v>1200</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="29">
         <v>435</v>
       </c>
       <c r="E4">
@@ -3318,7 +3316,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>3640</v>
@@ -3326,7 +3324,7 @@
       <c r="C5">
         <v>1200</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="29">
         <v>435</v>
       </c>
       <c r="E5">
@@ -3344,7 +3342,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>4250</v>
@@ -3373,7 +3371,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>995.2</v>
@@ -3381,6 +3379,9 @@
       <c r="C7">
         <v>294.3</v>
       </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
       <c r="E7">
         <v>700.9</v>
       </c>
@@ -3388,12 +3389,12 @@
         <v>0.7</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>1026</v>
@@ -3401,6 +3402,9 @@
       <c r="C8">
         <v>296</v>
       </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
       <c r="E8">
         <v>730</v>
       </c>
@@ -3408,12 +3412,12 @@
         <v>0.71</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>1039</v>
@@ -3421,6 +3425,9 @@
       <c r="C9">
         <v>306</v>
       </c>
+      <c r="D9">
+        <v>33</v>
+      </c>
       <c r="E9">
         <v>733</v>
       </c>
@@ -3428,12 +3435,12 @@
         <v>0.71</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>1006</v>
@@ -3441,6 +3448,9 @@
       <c r="C10">
         <v>299.60000000000002</v>
       </c>
+      <c r="D10">
+        <v>33</v>
+      </c>
       <c r="E10">
         <v>706.4</v>
       </c>
@@ -3448,12 +3458,12 @@
         <v>0.7</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <v>1006</v>
@@ -3461,6 +3471,9 @@
       <c r="C11">
         <v>303</v>
       </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
       <c r="E11">
         <v>703</v>
       </c>
@@ -3468,12 +3481,12 @@
         <v>0.7</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12">
         <v>585</v>
@@ -3493,7 +3506,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13">
         <v>1471</v>
@@ -3509,6 +3522,136 @@
       </c>
       <c r="H13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="8">
+        <v>93037</v>
+      </c>
+      <c r="C14" s="9">
+        <v>48886</v>
+      </c>
+      <c r="D14" s="10">
+        <v>48886</v>
+      </c>
+      <c r="E14" s="10">
+        <v>35894</v>
+      </c>
+      <c r="F14" s="10">
+        <v>44151</v>
+      </c>
+      <c r="G14" s="11">
+        <v>11198</v>
+      </c>
+      <c r="H14" s="10">
+        <v>307</v>
+      </c>
+      <c r="I14" s="10">
+        <v>385</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>1770</v>
+      </c>
+      <c r="L14" s="11">
+        <v>4969</v>
+      </c>
+      <c r="M14" s="8">
+        <v>266800</v>
+      </c>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60075</v>
+      </c>
+      <c r="C15" s="9">
+        <v>34823</v>
+      </c>
+      <c r="D15" s="10">
+        <v>34823</v>
+      </c>
+      <c r="E15" s="10">
+        <v>25000</v>
+      </c>
+      <c r="F15" s="10">
+        <v>25252</v>
+      </c>
+      <c r="G15" s="11">
+        <v>9823</v>
+      </c>
+      <c r="H15" s="10">
+        <v>898</v>
+      </c>
+      <c r="I15" s="10">
+        <v>478</v>
+      </c>
+      <c r="J15" s="10">
+        <v>2017</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1681</v>
+      </c>
+      <c r="L15" s="11">
+        <v>822</v>
+      </c>
+      <c r="M15" s="8">
+        <v>177929</v>
+      </c>
+      <c r="N15" s="8">
+        <v>177929</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="8">
+        <v>49972</v>
+      </c>
+      <c r="C16" s="8">
+        <v>19576</v>
+      </c>
+      <c r="D16" s="8">
+        <v>21929</v>
+      </c>
+      <c r="E16" s="8">
+        <v>14234</v>
+      </c>
+      <c r="F16" s="8">
+        <v>30396</v>
+      </c>
+      <c r="G16" s="8">
+        <v>9672</v>
+      </c>
+      <c r="H16" s="8">
+        <v>693</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1288</v>
+      </c>
+      <c r="J16" s="8">
+        <v>312</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1905</v>
+      </c>
+      <c r="L16" s="8">
+        <v>3036</v>
+      </c>
+      <c r="M16" s="8">
+        <v>44482.2</v>
+      </c>
+      <c r="N16" s="8">
+        <v>15568</v>
       </c>
     </row>
   </sheetData>
@@ -3522,7 +3665,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3545,7 +3688,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3554,54 +3697,54 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="8">
         <v>93037</v>
@@ -3643,7 +3786,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B3" s="8">
         <v>60075</v>
@@ -3687,7 +3830,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B4" s="8">
         <v>49972</v>

</xml_diff>

<commit_message>
corrections to plotter, and the DB
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conall De Paor\Desktop\Supaero\Research Project\Sizing-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7AA0A1-E5C1-46D7-A05E-95800DAA8876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B26C5E-2165-40AA-9C68-49114B27C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{A8CC2F8B-8671-446E-BE64-E520A416B0FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{A8CC2F8B-8671-446E-BE64-E520A416B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Swiss Cheese DB" sheetId="2" r:id="rId1"/>
     <sheet name="Manned Landers" sheetId="3" r:id="rId2"/>
-    <sheet name="Science Landers" sheetId="4" r:id="rId3"/>
-    <sheet name="Cargo Landers" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Science Landers" sheetId="4" r:id="rId4"/>
+    <sheet name="Cargo Landers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -236,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="108">
   <si>
     <t>Lander names</t>
   </si>
@@ -521,6 +522,45 @@
   </si>
   <si>
     <t>inert mass</t>
+  </si>
+  <si>
+    <t>wet mass</t>
+  </si>
+  <si>
+    <t>p/load</t>
+  </si>
+  <si>
+    <t>Tabulated data</t>
+  </si>
+  <si>
+    <t>Figure 7</t>
+  </si>
+  <si>
+    <t>drymass</t>
+  </si>
+  <si>
+    <t>Figure 8</t>
+  </si>
+  <si>
+    <t>Figure 9</t>
+  </si>
+  <si>
+    <t>Figure 5</t>
+  </si>
+  <si>
+    <t>Figure 6</t>
+  </si>
+  <si>
+    <t>Figure 10</t>
+  </si>
+  <si>
+    <t>Manned Landers</t>
+  </si>
+  <si>
+    <t>Spacecraft</t>
+  </si>
+  <si>
+    <t>Unmanned Landers</t>
   </si>
 </sst>
 </file>
@@ -552,7 +592,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,8 +611,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -755,11 +813,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -830,6 +1015,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2361,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F7DD18-26CD-4057-849D-39AE03A1CE0B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,6 +3398,770 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4530D16E-D44B-4BB8-BCE2-326DB78FCACB}">
+  <dimension ref="F11:N45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+    </row>
+    <row r="13" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+    </row>
+    <row r="14" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F14" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="49"/>
+      <c r="K14" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" s="51"/>
+    </row>
+    <row r="15" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="42"/>
+      <c r="G15" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="31">
+        <v>15103</v>
+      </c>
+      <c r="H16" s="46">
+        <v>4821</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4479</v>
+      </c>
+      <c r="J16" s="46">
+        <v>10624</v>
+      </c>
+      <c r="K16" s="31">
+        <v>15103</v>
+      </c>
+      <c r="L16" s="46">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="44">
+        <v>15065</v>
+      </c>
+      <c r="H17" s="47">
+        <v>4819</v>
+      </c>
+      <c r="I17" s="45">
+        <v>4214</v>
+      </c>
+      <c r="J17" s="47">
+        <v>10851</v>
+      </c>
+      <c r="K17" s="44">
+        <v>15065</v>
+      </c>
+      <c r="L17" s="47">
+        <v>4214</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="31">
+        <v>14916</v>
+      </c>
+      <c r="H18" s="46">
+        <v>4489</v>
+      </c>
+      <c r="I18" s="33">
+        <v>4226</v>
+      </c>
+      <c r="J18" s="46">
+        <v>10690</v>
+      </c>
+      <c r="K18" s="31">
+        <v>14916</v>
+      </c>
+      <c r="L18" s="46">
+        <v>4226</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="44">
+        <v>14916</v>
+      </c>
+      <c r="H19" s="47">
+        <v>4700</v>
+      </c>
+      <c r="I19" s="45">
+        <v>4284</v>
+      </c>
+      <c r="J19" s="47">
+        <v>10750</v>
+      </c>
+      <c r="K19" s="44">
+        <v>14916</v>
+      </c>
+      <c r="L19" s="47">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="31">
+        <v>16447</v>
+      </c>
+      <c r="H20" s="46">
+        <v>4795</v>
+      </c>
+      <c r="I20" s="33">
+        <v>5113</v>
+      </c>
+      <c r="J20" s="46">
+        <v>11019</v>
+      </c>
+      <c r="K20" s="31">
+        <v>16447</v>
+      </c>
+      <c r="L20" s="46">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="44">
+        <v>16447</v>
+      </c>
+      <c r="H21" s="47">
+        <v>4795</v>
+      </c>
+      <c r="I21" s="45">
+        <v>5113</v>
+      </c>
+      <c r="J21" s="47">
+        <v>11019</v>
+      </c>
+      <c r="K21" s="44">
+        <v>16447</v>
+      </c>
+      <c r="L21" s="47">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="31">
+        <v>16447</v>
+      </c>
+      <c r="H22" s="46">
+        <v>4795</v>
+      </c>
+      <c r="I22" s="33">
+        <v>5113</v>
+      </c>
+      <c r="J22" s="46">
+        <v>11019</v>
+      </c>
+      <c r="K22" s="31">
+        <v>16447</v>
+      </c>
+      <c r="L22" s="46">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="44">
+        <v>93038</v>
+      </c>
+      <c r="H23" s="47">
+        <v>31384</v>
+      </c>
+      <c r="I23" s="45">
+        <v>29403</v>
+      </c>
+      <c r="J23" s="47">
+        <v>62458</v>
+      </c>
+      <c r="K23" s="44">
+        <v>93038</v>
+      </c>
+      <c r="L23" s="47">
+        <v>29403</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="31">
+        <v>48218</v>
+      </c>
+      <c r="H24" s="46">
+        <v>6000</v>
+      </c>
+      <c r="I24" s="33">
+        <v>15823</v>
+      </c>
+      <c r="J24" s="46">
+        <v>32395</v>
+      </c>
+      <c r="K24" s="31">
+        <v>48218</v>
+      </c>
+      <c r="L24" s="46">
+        <v>15823</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F25" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="44">
+        <v>5038.6000000000004</v>
+      </c>
+      <c r="H25" s="47">
+        <v>473</v>
+      </c>
+      <c r="I25" s="45">
+        <v>1673.7</v>
+      </c>
+      <c r="J25" s="47">
+        <v>3223.8</v>
+      </c>
+      <c r="K25" s="44">
+        <v>5038.6000000000004</v>
+      </c>
+      <c r="L25" s="47">
+        <v>1673.7</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="31">
+        <v>45862</v>
+      </c>
+      <c r="H26" s="46">
+        <v>14135</v>
+      </c>
+      <c r="I26" s="33">
+        <v>15425</v>
+      </c>
+      <c r="J26" s="46">
+        <v>29820</v>
+      </c>
+      <c r="K26" s="31">
+        <v>45862</v>
+      </c>
+      <c r="L26" s="46">
+        <v>15425</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="32">
+        <v>81911</v>
+      </c>
+      <c r="H27" s="48">
+        <v>10790</v>
+      </c>
+      <c r="I27" s="34">
+        <v>26912</v>
+      </c>
+      <c r="J27" s="48">
+        <v>54360</v>
+      </c>
+      <c r="K27" s="32">
+        <v>81911</v>
+      </c>
+      <c r="L27" s="48">
+        <v>26912</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="38"/>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F29" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="41"/>
+      <c r="I29" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29" s="41"/>
+      <c r="K29" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="L29" s="41"/>
+    </row>
+    <row r="30" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="42"/>
+      <c r="G30" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K30" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="L30" s="53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F31" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="31">
+        <v>5750</v>
+      </c>
+      <c r="H31" s="46">
+        <v>1880</v>
+      </c>
+      <c r="I31" s="33">
+        <v>5750</v>
+      </c>
+      <c r="J31" s="46">
+        <v>1880</v>
+      </c>
+      <c r="K31" s="31">
+        <v>5750</v>
+      </c>
+      <c r="L31" s="46">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F32" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="44">
+        <v>5700</v>
+      </c>
+      <c r="H32" s="47">
+        <v>1814</v>
+      </c>
+      <c r="I32" s="45">
+        <v>5700</v>
+      </c>
+      <c r="J32" s="47">
+        <v>1814</v>
+      </c>
+      <c r="K32" s="44">
+        <v>5700</v>
+      </c>
+      <c r="L32" s="47">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F33" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="31">
+        <v>3780</v>
+      </c>
+      <c r="H33" s="46">
+        <v>1200</v>
+      </c>
+      <c r="I33" s="33">
+        <v>3780</v>
+      </c>
+      <c r="J33" s="46">
+        <v>1200</v>
+      </c>
+      <c r="K33" s="31">
+        <v>3780</v>
+      </c>
+      <c r="L33" s="46">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F34" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="44">
+        <v>3640</v>
+      </c>
+      <c r="H34" s="47">
+        <v>1200</v>
+      </c>
+      <c r="I34" s="45">
+        <v>3640</v>
+      </c>
+      <c r="J34" s="47">
+        <v>1200</v>
+      </c>
+      <c r="K34" s="44">
+        <v>3640</v>
+      </c>
+      <c r="L34" s="47">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F35" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="31">
+        <v>4250</v>
+      </c>
+      <c r="H35" s="46">
+        <v>1497</v>
+      </c>
+      <c r="I35" s="33">
+        <v>4250</v>
+      </c>
+      <c r="J35" s="46">
+        <v>1497</v>
+      </c>
+      <c r="K35" s="31">
+        <v>4250</v>
+      </c>
+      <c r="L35" s="46">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F36" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="44">
+        <v>995.2</v>
+      </c>
+      <c r="H36" s="47">
+        <v>294.3</v>
+      </c>
+      <c r="I36" s="45">
+        <v>995.2</v>
+      </c>
+      <c r="J36" s="47">
+        <v>294.3</v>
+      </c>
+      <c r="K36" s="44">
+        <v>995.2</v>
+      </c>
+      <c r="L36" s="47">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F37" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="31">
+        <v>1026</v>
+      </c>
+      <c r="H37" s="46">
+        <v>296</v>
+      </c>
+      <c r="I37" s="33">
+        <v>1026</v>
+      </c>
+      <c r="J37" s="46">
+        <v>296</v>
+      </c>
+      <c r="K37" s="31">
+        <v>1026</v>
+      </c>
+      <c r="L37" s="46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F38" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="44">
+        <v>1039</v>
+      </c>
+      <c r="H38" s="47">
+        <v>306</v>
+      </c>
+      <c r="I38" s="45">
+        <v>1039</v>
+      </c>
+      <c r="J38" s="47">
+        <v>306</v>
+      </c>
+      <c r="K38" s="44">
+        <v>1039</v>
+      </c>
+      <c r="L38" s="47">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F39" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="31">
+        <v>1006</v>
+      </c>
+      <c r="H39" s="46">
+        <v>299.60000000000002</v>
+      </c>
+      <c r="I39" s="33">
+        <v>1006</v>
+      </c>
+      <c r="J39" s="46">
+        <v>299.60000000000002</v>
+      </c>
+      <c r="K39" s="31">
+        <v>1006</v>
+      </c>
+      <c r="L39" s="46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F40" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="44">
+        <v>1006</v>
+      </c>
+      <c r="H40" s="47">
+        <v>303</v>
+      </c>
+      <c r="I40" s="45">
+        <v>1006</v>
+      </c>
+      <c r="J40" s="47">
+        <v>303</v>
+      </c>
+      <c r="K40" s="44">
+        <v>1006</v>
+      </c>
+      <c r="L40" s="47">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="31">
+        <v>585</v>
+      </c>
+      <c r="H41" s="46">
+        <v>150</v>
+      </c>
+      <c r="I41" s="33">
+        <v>585</v>
+      </c>
+      <c r="J41" s="46">
+        <v>150</v>
+      </c>
+      <c r="K41" s="31">
+        <v>585</v>
+      </c>
+      <c r="L41" s="46"/>
+    </row>
+    <row r="42" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F42" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="44">
+        <v>1471</v>
+      </c>
+      <c r="H42" s="47">
+        <v>626</v>
+      </c>
+      <c r="I42" s="45">
+        <v>1471</v>
+      </c>
+      <c r="J42" s="47">
+        <v>626</v>
+      </c>
+      <c r="K42" s="44">
+        <v>1471</v>
+      </c>
+      <c r="L42" s="47"/>
+    </row>
+    <row r="43" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F43" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="31">
+        <v>93037</v>
+      </c>
+      <c r="H43" s="46">
+        <v>48886</v>
+      </c>
+      <c r="I43" s="33">
+        <v>93037</v>
+      </c>
+      <c r="J43" s="46">
+        <v>48886</v>
+      </c>
+      <c r="K43" s="31">
+        <v>93037</v>
+      </c>
+      <c r="L43" s="46">
+        <v>48886</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F44" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="44">
+        <v>60075</v>
+      </c>
+      <c r="H44" s="47">
+        <v>34823</v>
+      </c>
+      <c r="I44" s="45">
+        <v>60075</v>
+      </c>
+      <c r="J44" s="47">
+        <v>34823</v>
+      </c>
+      <c r="K44" s="44">
+        <v>60075</v>
+      </c>
+      <c r="L44" s="47">
+        <v>34823</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="32">
+        <v>49972</v>
+      </c>
+      <c r="H45" s="48">
+        <v>19576</v>
+      </c>
+      <c r="I45" s="34">
+        <v>49972</v>
+      </c>
+      <c r="J45" s="48">
+        <v>19576</v>
+      </c>
+      <c r="K45" s="32">
+        <v>49972</v>
+      </c>
+      <c r="L45" s="48">
+        <v>21929</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="F13:L13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="K14:L14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80C5C0-5165-4D8F-8D34-D728F416EF6B}">
   <dimension ref="A1:N16"/>
   <sheetViews>
@@ -3660,7 +4656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77947650-EFE6-4BC5-8EC3-7F1726132A86}">
   <dimension ref="A1:U4"/>
   <sheetViews>

</xml_diff>

<commit_message>
plots now have colours, and equation of the line in the legend
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conall De Paor\Desktop\Supaero\Research Project\Sizing-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B26C5E-2165-40AA-9C68-49114B27C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76645FEA-44E9-4121-8D7A-FE52506E644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{A8CC2F8B-8671-446E-BE64-E520A416B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Swiss Cheese DB" sheetId="2" r:id="rId1"/>
     <sheet name="Manned Landers" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="Science Landers" sheetId="4" r:id="rId4"/>
-    <sheet name="Cargo Landers" sheetId="5" r:id="rId5"/>
+    <sheet name="Science Landers" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="export sheet" sheetId="7" r:id="rId5"/>
+    <sheet name="Cargo Landers" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -236,8 +237,76 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Conall De Paor</author>
+  </authors>
+  <commentList>
+    <comment ref="H51" authorId="0" shapeId="0" xr:uid="{1DBD8923-8291-4CE8-86B9-6AB6835F395F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Conall De Paor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+dry mass is equivalent to landed mass for oneway science rovers</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Conall De Paor</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{925642B3-B3FE-4FAC-B22C-C166687C1C78}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Conall De Paor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CEV</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="112">
   <si>
     <t>Lander names</t>
   </si>
@@ -561,6 +630,18 @@
   </si>
   <si>
     <t>Unmanned Landers</t>
+  </si>
+  <si>
+    <t>0507-ESAS-F</t>
+  </si>
+  <si>
+    <t>0507-ESAS-F Cargo</t>
+  </si>
+  <si>
+    <t>Ye-8</t>
+  </si>
+  <si>
+    <t>Ye-8-5M</t>
   </si>
 </sst>
 </file>
@@ -592,7 +673,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,12 +683,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,7 +705,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -940,11 +1015,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1014,54 +1124,73 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,6 +1206,1093 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18888670166229221"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.76911329833770781"/>
+          <c:h val="0.63759988334791484"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.0930008748906389E-2"/>
+                  <c:y val="0.26558982210557014"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$31:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3820</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2580</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2440</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2753</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>706.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>703</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$31:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.56119402985074629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47486910994764397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46511627906976744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49180327868852458</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54377043225572108</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41988871450991583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40547945205479452</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.417462482946794</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4241223103057758</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43100995732574682</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.34482758620689657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.74082840236686387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-30D1-4FFF-B94E-A1EE59F9D78D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="651510792"/>
+        <c:axId val="651507184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="651510792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651507184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="651507184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651510792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.1309959711192328E-4"/>
+          <c:y val="0.87982362692640625"/>
+          <c:w val="0.48055997281214924"/>
+          <c:h val="7.8116832986696597E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>578191</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>58920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>16522</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80997</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA06AE4-E493-DB75-0B62-8B3B7F399F32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2594,7 +3810,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A8" sqref="A8:U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,752 +4614,2205 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4530D16E-D44B-4BB8-BCE2-326DB78FCACB}">
-  <dimension ref="F11:N45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80C5C0-5165-4D8F-8D34-D728F416EF6B}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>5750</v>
+      </c>
+      <c r="C2">
+        <v>1880</v>
+      </c>
+      <c r="D2">
+        <v>512</v>
+      </c>
+      <c r="E2">
+        <v>3350</v>
+      </c>
+      <c r="F2">
+        <v>1880</v>
+      </c>
+      <c r="G2" s="59">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H2">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>5700</v>
+      </c>
+      <c r="C3">
+        <v>1814</v>
+      </c>
+      <c r="D3">
+        <v>756</v>
+      </c>
+      <c r="E3">
+        <v>3820</v>
+      </c>
+      <c r="F3">
+        <v>1058</v>
+      </c>
+      <c r="G3" s="59">
+        <v>0.67</v>
+      </c>
+      <c r="H3">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>3780</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+      <c r="D4" s="67">
+        <v>435</v>
+      </c>
+      <c r="E4">
+        <v>2580</v>
+      </c>
+      <c r="F4">
+        <v>765</v>
+      </c>
+      <c r="G4" s="59">
+        <v>0.68</v>
+      </c>
+      <c r="H4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>3640</v>
+      </c>
+      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="67">
+        <v>435</v>
+      </c>
+      <c r="E5">
+        <v>2440</v>
+      </c>
+      <c r="F5">
+        <v>765</v>
+      </c>
+      <c r="G5" s="59">
+        <v>0.67</v>
+      </c>
+      <c r="H5">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>4250</v>
+      </c>
+      <c r="C6">
+        <v>1497</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>2753</v>
+      </c>
+      <c r="F6">
+        <v>1197</v>
+      </c>
+      <c r="G6" s="59">
+        <v>0.65</v>
+      </c>
+      <c r="H6">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="J6">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>995.2</v>
+      </c>
+      <c r="C7">
+        <v>294.3</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>700.9</v>
+      </c>
+      <c r="F7">
+        <v>261.3</v>
+      </c>
+      <c r="G7">
+        <v>0.7</v>
+      </c>
+      <c r="H7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>1026</v>
+      </c>
+      <c r="C8">
+        <v>296</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>730</v>
+      </c>
+      <c r="G8">
+        <v>0.71</v>
+      </c>
+      <c r="H8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>1039</v>
+      </c>
+      <c r="C9">
+        <v>306</v>
+      </c>
+      <c r="D9">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>733</v>
+      </c>
+      <c r="G9">
+        <v>0.71</v>
+      </c>
+      <c r="H9">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>1006</v>
+      </c>
+      <c r="C10">
+        <v>299.60000000000002</v>
+      </c>
+      <c r="D10">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>706.4</v>
+      </c>
+      <c r="G10">
+        <v>0.7</v>
+      </c>
+      <c r="H10">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>1006</v>
+      </c>
+      <c r="C11">
+        <v>303</v>
+      </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>703</v>
+      </c>
+      <c r="G11">
+        <v>0.7</v>
+      </c>
+      <c r="H11">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>585</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="E12">
+        <v>435</v>
+      </c>
+      <c r="G12">
+        <v>0.74</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>1471</v>
+      </c>
+      <c r="C13">
+        <v>626</v>
+      </c>
+      <c r="E13">
+        <v>845</v>
+      </c>
+      <c r="G13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="8">
+        <v>93037</v>
+      </c>
+      <c r="C14" s="9">
+        <v>48886</v>
+      </c>
+      <c r="D14" s="10">
+        <v>37628</v>
+      </c>
+      <c r="E14" s="10">
+        <v>44151</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10">
+        <v>307</v>
+      </c>
+      <c r="I14" s="10">
+        <v>385</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>1770</v>
+      </c>
+      <c r="L14" s="11">
+        <v>4969</v>
+      </c>
+      <c r="M14" s="8">
+        <v>266800</v>
+      </c>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60075</v>
+      </c>
+      <c r="C15" s="9">
+        <v>34823</v>
+      </c>
+      <c r="D15" s="10">
+        <v>25000</v>
+      </c>
+      <c r="E15" s="10">
+        <v>25252</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10">
+        <v>898</v>
+      </c>
+      <c r="I15" s="10">
+        <v>478</v>
+      </c>
+      <c r="J15" s="10">
+        <v>2017</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1681</v>
+      </c>
+      <c r="L15" s="11">
+        <v>822</v>
+      </c>
+      <c r="M15" s="8">
+        <v>177929</v>
+      </c>
+      <c r="N15" s="8">
+        <v>177929</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="8">
+        <v>45001</v>
+      </c>
+      <c r="C16" s="8">
+        <v>16958</v>
+      </c>
+      <c r="D16" s="8">
+        <v>6532</v>
+      </c>
+      <c r="E16" s="8">
+        <v>28043</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8">
+        <v>693</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1288</v>
+      </c>
+      <c r="J16" s="8">
+        <v>312</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1905</v>
+      </c>
+      <c r="L16" s="8">
+        <v>3036</v>
+      </c>
+      <c r="M16" s="8">
+        <v>44482.2</v>
+      </c>
+      <c r="N16" s="8">
+        <v>15568</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="18">
+        <v>28819</v>
+      </c>
+      <c r="C17" s="18">
+        <v>9667</v>
+      </c>
+      <c r="D17" s="8">
+        <v>6532</v>
+      </c>
+      <c r="E17" s="8">
+        <v>19152</v>
+      </c>
+      <c r="F17" s="8">
+        <v>7695</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4530D16E-D44B-4BB8-BCE2-326DB78FCACB}">
+  <dimension ref="F11:W55"/>
+  <sheetViews>
+    <sheetView topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="36" t="s">
+    <row r="11" spans="6:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="6:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-    </row>
-    <row r="13" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="36" t="s">
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+    </row>
+    <row r="13" spans="6:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-    </row>
-    <row r="14" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F14" s="39" t="s">
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F14" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="47"/>
+      <c r="I14" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="49" t="s">
+      <c r="J14" s="53"/>
+      <c r="K14" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="55"/>
+      <c r="O14" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="49"/>
-      <c r="K14" s="50" t="s">
+      <c r="P14" s="47"/>
+      <c r="Q14" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="53"/>
+      <c r="S14" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="51"/>
-    </row>
-    <row r="15" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="42"/>
-      <c r="G15" s="52" t="s">
+      <c r="T14" s="55"/>
+    </row>
+    <row r="15" spans="6:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="49"/>
+      <c r="G15" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="53" t="s">
+      <c r="H15" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="53" t="s">
+      <c r="J15" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="52" t="s">
+      <c r="K15" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="L15" s="53" t="s">
+      <c r="L15" s="42" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="P15" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q15" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="R15" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="T15" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="30">
         <v>15103</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="38">
         <v>4821</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="32">
         <v>4479</v>
       </c>
-      <c r="J16" s="46">
+      <c r="J16" s="38">
         <v>10624</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="30">
         <v>15103</v>
       </c>
-      <c r="L16" s="46">
+      <c r="L16" s="38">
         <v>4479</v>
       </c>
-    </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F17" s="43" t="s">
+      <c r="O16">
+        <f>G16/G16</f>
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <f>H16/G16</f>
+        <v>0.31920810435012914</v>
+      </c>
+      <c r="Q16">
+        <f>I16/I16</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="59">
+        <f>I16/J16</f>
+        <v>0.42159262048192769</v>
+      </c>
+      <c r="S16">
+        <f>K16/K16</f>
+        <v>1</v>
+      </c>
+      <c r="T16" s="59">
+        <f>L16/K16</f>
+        <v>0.29656359663642984</v>
+      </c>
+    </row>
+    <row r="17" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F17" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="44">
+      <c r="G17" s="36">
         <v>15065</v>
       </c>
-      <c r="H17" s="47">
+      <c r="H17" s="39">
         <v>4819</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I17" s="37">
         <v>4214</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="39">
         <v>10851</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="36">
         <v>15065</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="39">
         <v>4214</v>
       </c>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f t="shared" ref="O17:O27" si="0">G17/G17</f>
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P27" si="1">H17/G17</f>
+        <v>0.31988051775638898</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ref="Q17:Q27" si="2">I17/I17</f>
+        <v>1</v>
+      </c>
+      <c r="R17" s="59">
+        <f t="shared" ref="R17:R27" si="3">I17/J17</f>
+        <v>0.38835130402727858</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17:S27" si="4">K17/K17</f>
+        <v>1</v>
+      </c>
+      <c r="T17" s="59">
+        <f t="shared" ref="T17:T27" si="5">L17/K17</f>
+        <v>0.27972120809824097</v>
+      </c>
+    </row>
+    <row r="18" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="30">
         <v>14916</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="38">
         <v>4489</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="32">
         <v>4226</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="38">
         <v>10690</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="30">
         <v>14916</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="38">
         <v>4226</v>
       </c>
-    </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="43" t="s">
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>0.30095199785465271</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R18" s="59">
+        <f t="shared" si="3"/>
+        <v>0.39532273152478953</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T18" s="59">
+        <f t="shared" si="5"/>
+        <v>0.28331992491284524</v>
+      </c>
+    </row>
+    <row r="19" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="44">
+      <c r="G19" s="36">
         <v>14916</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="39">
         <v>4700</v>
       </c>
-      <c r="I19" s="45">
+      <c r="I19" s="37">
         <v>4284</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="39">
         <v>10750</v>
       </c>
-      <c r="K19" s="44">
+      <c r="K19" s="36">
         <v>14916</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="39">
         <v>4284</v>
       </c>
-    </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="1"/>
+        <v>0.31509788146956291</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R19" s="59">
+        <f t="shared" si="3"/>
+        <v>0.39851162790697675</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T19" s="59">
+        <f t="shared" si="5"/>
+        <v>0.28720836685438456</v>
+      </c>
+    </row>
+    <row r="20" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="30">
         <v>16447</v>
       </c>
-      <c r="H20" s="46">
+      <c r="H20" s="38">
         <v>4795</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="32">
         <v>5113</v>
       </c>
-      <c r="J20" s="46">
+      <c r="J20" s="38">
         <v>11019</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="30">
         <v>16447</v>
       </c>
-      <c r="L20" s="46">
+      <c r="L20" s="38">
         <v>5113</v>
       </c>
-    </row>
-    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="43" t="s">
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
+        <v>0.29154253055268436</v>
+      </c>
+      <c r="Q20">
+        <f>I20/I20</f>
+        <v>1</v>
+      </c>
+      <c r="R20" s="59">
+        <f t="shared" si="3"/>
+        <v>0.46401669842998455</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T20" s="59">
+        <f t="shared" si="5"/>
+        <v>0.31087736365294583</v>
+      </c>
+    </row>
+    <row r="21" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F21" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="44">
+      <c r="G21" s="36">
         <v>16447</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="39">
         <v>4795</v>
       </c>
-      <c r="I21" s="45">
+      <c r="I21" s="37">
         <v>5113</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="39">
         <v>11019</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="36">
         <v>16447</v>
       </c>
-      <c r="L21" s="47">
+      <c r="L21" s="39">
         <v>5113</v>
       </c>
-    </row>
-    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
+        <v>0.29154253055268436</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="59">
+        <f t="shared" si="3"/>
+        <v>0.46401669842998455</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T21" s="59">
+        <f t="shared" si="5"/>
+        <v>0.31087736365294583</v>
+      </c>
+    </row>
+    <row r="22" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="30">
         <v>16447</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="38">
         <v>4795</v>
       </c>
-      <c r="I22" s="33">
+      <c r="I22" s="32">
         <v>5113</v>
       </c>
-      <c r="J22" s="46">
+      <c r="J22" s="38">
         <v>11019</v>
       </c>
-      <c r="K22" s="31">
+      <c r="K22" s="30">
         <v>16447</v>
       </c>
-      <c r="L22" s="46">
+      <c r="L22" s="38">
         <v>5113</v>
       </c>
-    </row>
-    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="43" t="s">
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>0.29154253055268436</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R22" s="59">
+        <f t="shared" si="3"/>
+        <v>0.46401669842998455</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T22" s="59">
+        <f t="shared" si="5"/>
+        <v>0.31087736365294583</v>
+      </c>
+    </row>
+    <row r="23" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F23" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="36">
         <v>93038</v>
       </c>
-      <c r="H23" s="47">
+      <c r="H23" s="39">
         <v>31384</v>
       </c>
-      <c r="I23" s="45">
+      <c r="I23" s="37">
         <v>29403</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="39">
         <v>62458</v>
       </c>
-      <c r="K23" s="44">
+      <c r="K23" s="36">
         <v>93038</v>
       </c>
-      <c r="L23" s="47">
+      <c r="L23" s="39">
         <v>29403</v>
       </c>
-    </row>
-    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>0.33732453406135127</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R23" s="59">
+        <f t="shared" si="3"/>
+        <v>0.47076435364564989</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T23" s="59">
+        <f t="shared" si="5"/>
+        <v>0.31603215890281389</v>
+      </c>
+    </row>
+    <row r="24" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="31">
+      <c r="G24" s="30">
         <v>48218</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="38">
         <v>6000</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="32">
         <v>15823</v>
       </c>
-      <c r="J24" s="46">
+      <c r="J24" s="38">
         <v>32395</v>
       </c>
-      <c r="K24" s="31">
+      <c r="K24" s="30">
         <v>48218</v>
       </c>
-      <c r="L24" s="46">
+      <c r="L24" s="38">
         <v>15823</v>
       </c>
-    </row>
-    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="43" t="s">
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>0.12443485835165291</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R24" s="59">
+        <f t="shared" si="3"/>
+        <v>0.4884395740083346</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T24" s="59">
+        <f t="shared" si="5"/>
+        <v>0.32815546061636736</v>
+      </c>
+    </row>
+    <row r="25" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F25" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="44">
+      <c r="G25" s="36">
         <v>5038.6000000000004</v>
       </c>
-      <c r="H25" s="47">
+      <c r="H25" s="39">
         <v>473</v>
       </c>
-      <c r="I25" s="45">
+      <c r="I25" s="37">
         <v>1673.7</v>
       </c>
-      <c r="J25" s="47">
+      <c r="J25" s="39">
         <v>3223.8</v>
       </c>
-      <c r="K25" s="44">
+      <c r="K25" s="36">
         <v>5038.6000000000004</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="39">
         <v>1673.7</v>
       </c>
-    </row>
-    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>9.3875282816655414E-2</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R25" s="59">
+        <f t="shared" si="3"/>
+        <v>0.51916992369253678</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T25" s="59">
+        <f t="shared" si="5"/>
+        <v>0.33217560433453736</v>
+      </c>
+    </row>
+    <row r="26" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F26" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="30">
         <v>45862</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H26" s="38">
         <v>14135</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="32">
         <v>15425</v>
       </c>
-      <c r="J26" s="46">
+      <c r="J26" s="38">
         <v>29820</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="30">
         <v>45862</v>
       </c>
-      <c r="L26" s="46">
+      <c r="L26" s="38">
         <v>15425</v>
       </c>
-    </row>
-    <row r="27" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="35" t="s">
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>0.30820723038681264</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R26" s="59">
+        <f t="shared" si="3"/>
+        <v>0.51727028839704892</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T26" s="59">
+        <f t="shared" si="5"/>
+        <v>0.33633509223322139</v>
+      </c>
+    </row>
+    <row r="27" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="31">
         <v>81911</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="40">
         <v>10790</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="33">
         <v>26912</v>
       </c>
-      <c r="J27" s="48">
+      <c r="J27" s="40">
         <v>54360</v>
       </c>
-      <c r="K27" s="32">
+      <c r="K27" s="31">
         <v>81911</v>
       </c>
-      <c r="L27" s="48">
+      <c r="L27" s="40">
         <v>26912</v>
       </c>
-    </row>
-    <row r="28" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="36" t="s">
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>0.13172833929508856</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R27" s="59">
+        <f t="shared" si="3"/>
+        <v>0.4950699043414275</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T27" s="59">
+        <f t="shared" si="5"/>
+        <v>0.32855172077010414</v>
+      </c>
+    </row>
+    <row r="28" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
-    </row>
-    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="39" t="s">
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="52"/>
+      <c r="P28">
+        <f>AVERAGE(P16:P27)</f>
+        <v>0.26044469483336236</v>
+      </c>
+      <c r="R28" s="59">
+        <f>AVERAGE(R16:R27)</f>
+        <v>0.4572118686096604</v>
+      </c>
+      <c r="T28" s="59">
+        <f>AVERAGE(T16:T27)</f>
+        <v>0.31005793535981524</v>
+      </c>
+    </row>
+    <row r="29" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F29" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="H29" s="41"/>
-      <c r="I29" s="40" t="s">
+      <c r="G29" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="40" t="s">
+      <c r="J29" s="47"/>
+      <c r="K29" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="L29" s="41"/>
-    </row>
-    <row r="30" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="42"/>
-      <c r="G30" s="52" t="s">
+      <c r="L29" s="47"/>
+      <c r="O29" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="R29" s="47"/>
+      <c r="S29" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="T29" s="47"/>
+    </row>
+    <row r="30" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="49"/>
+      <c r="G30" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="H30" s="53" t="s">
+      <c r="H30" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I30" s="54" t="s">
+      <c r="K30" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="L30" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="O30" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="P30" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q30" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="J30" s="53" t="s">
+      <c r="R30" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="K30" s="55" t="s">
+      <c r="S30" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="L30" s="53" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="31" t="s">
+      <c r="T30" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F31" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="31">
+      <c r="G31" s="30">
         <v>5750</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="38">
+        <v>512</v>
+      </c>
+      <c r="I31" s="56">
+        <v>3350</v>
+      </c>
+      <c r="J31" s="38">
         <v>1880</v>
       </c>
-      <c r="I31" s="33">
+      <c r="K31" s="30">
         <v>5750</v>
       </c>
-      <c r="J31" s="46">
+      <c r="L31" s="38">
         <v>1880</v>
       </c>
-      <c r="K31" s="31">
-        <v>5750</v>
-      </c>
-      <c r="L31" s="46">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="43" t="s">
+      <c r="O31">
+        <f>G31/G31</f>
+        <v>1</v>
+      </c>
+      <c r="P31" s="59">
+        <f>H31/G31</f>
+        <v>8.9043478260869571E-2</v>
+      </c>
+      <c r="Q31">
+        <f>I31/I31</f>
+        <v>1</v>
+      </c>
+      <c r="R31" s="59">
+        <f>J31/I31</f>
+        <v>0.56119402985074629</v>
+      </c>
+      <c r="S31">
+        <f>K31/K31</f>
+        <v>1</v>
+      </c>
+      <c r="T31" s="59">
+        <f>1/(K31/L31)</f>
+        <v>0.32695652173913042</v>
+      </c>
+    </row>
+    <row r="32" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F32" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="36">
         <v>5700</v>
       </c>
-      <c r="H32" s="47">
+      <c r="H32" s="39">
+        <v>756</v>
+      </c>
+      <c r="I32" s="57">
+        <v>3820</v>
+      </c>
+      <c r="J32" s="39">
         <v>1814</v>
       </c>
-      <c r="I32" s="45">
+      <c r="K32" s="36">
         <v>5700</v>
       </c>
-      <c r="J32" s="47">
+      <c r="L32" s="39">
         <v>1814</v>
       </c>
-      <c r="K32" s="44">
-        <v>5700</v>
-      </c>
-      <c r="L32" s="47">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f t="shared" ref="O32:O45" si="6">G32/G32</f>
+        <v>1</v>
+      </c>
+      <c r="P32" s="59">
+        <f t="shared" ref="P32:P45" si="7">H32/G32</f>
+        <v>0.13263157894736843</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ref="Q32:Q46" si="8">I32/I32</f>
+        <v>1</v>
+      </c>
+      <c r="R32" s="59">
+        <f t="shared" ref="R32:R45" si="9">J32/I32</f>
+        <v>0.47486910994764397</v>
+      </c>
+      <c r="S32">
+        <f t="shared" ref="S32:S46" si="10">K32/K32</f>
+        <v>1</v>
+      </c>
+      <c r="T32" s="59">
+        <f t="shared" ref="T32:T45" si="11">1/(K32/L32)</f>
+        <v>0.31824561403508772</v>
+      </c>
+      <c r="V32" s="36">
+        <v>60075</v>
+      </c>
+      <c r="W32">
+        <v>1.7251529161760906</v>
+      </c>
+    </row>
+    <row r="33" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F33" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="31">
+      <c r="G33" s="30">
         <v>3780</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="38">
+        <v>435</v>
+      </c>
+      <c r="I33" s="56">
+        <v>2580</v>
+      </c>
+      <c r="J33" s="38">
         <v>1200</v>
       </c>
-      <c r="I33" s="33">
+      <c r="K33" s="30">
         <v>3780</v>
       </c>
-      <c r="J33" s="46">
+      <c r="L33" s="38">
         <v>1200</v>
       </c>
-      <c r="K33" s="31">
-        <v>3780</v>
-      </c>
-      <c r="L33" s="46">
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P33" s="59">
+        <f t="shared" si="7"/>
+        <v>0.11507936507936507</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="59">
+        <f t="shared" si="9"/>
+        <v>0.46511627906976744</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T33" s="59">
+        <f t="shared" si="11"/>
+        <v>0.31746031746031744</v>
+      </c>
+      <c r="V33" s="36">
+        <v>1039</v>
+      </c>
+      <c r="W33">
+        <v>31.484848484848484</v>
+      </c>
+    </row>
+    <row r="34" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F34" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="36">
+        <v>3640</v>
+      </c>
+      <c r="H34" s="39">
         <v>435</v>
       </c>
-    </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F34" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="44">
+      <c r="I34" s="57">
+        <v>2440</v>
+      </c>
+      <c r="J34" s="39">
+        <v>1200</v>
+      </c>
+      <c r="K34" s="36">
         <v>3640</v>
       </c>
-      <c r="H34" s="47">
+      <c r="L34" s="39">
         <v>1200</v>
       </c>
-      <c r="I34" s="45">
-        <v>3640</v>
-      </c>
-      <c r="J34" s="47">
-        <v>1200</v>
-      </c>
-      <c r="K34" s="44">
-        <v>3640</v>
-      </c>
-      <c r="L34" s="47">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P34" s="59">
+        <f t="shared" si="7"/>
+        <v>0.11950549450549451</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R34" s="59">
+        <f t="shared" si="9"/>
+        <v>0.49180327868852458</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T34" s="59">
+        <f t="shared" si="11"/>
+        <v>0.32967032967032966</v>
+      </c>
+      <c r="V34" s="30">
+        <v>1026</v>
+      </c>
+      <c r="W34">
+        <v>31.09090909090909</v>
+      </c>
+    </row>
+    <row r="35" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F35" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="31">
+      <c r="G35" s="30">
         <v>4250</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="38">
+        <v>300</v>
+      </c>
+      <c r="I35" s="56">
+        <v>2753</v>
+      </c>
+      <c r="J35" s="38">
         <v>1497</v>
       </c>
-      <c r="I35" s="33">
+      <c r="K35" s="30">
         <v>4250</v>
       </c>
-      <c r="J35" s="46">
+      <c r="L35" s="38">
         <v>1497</v>
       </c>
-      <c r="K35" s="31">
-        <v>4250</v>
-      </c>
-      <c r="L35" s="46">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F36" s="43" t="s">
+      <c r="O35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="59">
+        <f t="shared" si="7"/>
+        <v>7.0588235294117646E-2</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R35" s="59">
+        <f t="shared" si="9"/>
+        <v>0.54377043225572108</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T35" s="59">
+        <f t="shared" si="11"/>
+        <v>0.35223529411764709</v>
+      </c>
+      <c r="V35" s="30">
+        <v>1006</v>
+      </c>
+      <c r="W35">
+        <v>30.484848484848484</v>
+      </c>
+    </row>
+    <row r="36" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F36" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="44">
+      <c r="G36" s="36">
         <v>995.2</v>
       </c>
-      <c r="H36" s="47">
+      <c r="H36" s="39">
+        <v>33</v>
+      </c>
+      <c r="I36" s="57">
+        <v>700.9</v>
+      </c>
+      <c r="J36" s="39">
         <v>294.3</v>
       </c>
-      <c r="I36" s="45">
+      <c r="K36" s="36">
         <v>995.2</v>
       </c>
-      <c r="J36" s="47">
+      <c r="L36" s="39">
         <v>294.3</v>
       </c>
-      <c r="K36" s="44">
-        <v>995.2</v>
-      </c>
-      <c r="L36" s="47">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P36" s="59">
+        <f t="shared" si="7"/>
+        <v>3.3159163987138265E-2</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R36" s="59">
+        <f t="shared" si="9"/>
+        <v>0.41988871450991583</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T36" s="59">
+        <f t="shared" si="11"/>
+        <v>0.29571945337620575</v>
+      </c>
+      <c r="V36" s="36">
+        <v>1006</v>
+      </c>
+      <c r="W36">
+        <v>30.484848484848484</v>
+      </c>
+    </row>
+    <row r="37" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F37" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G37" s="31">
+      <c r="G37" s="30">
         <v>1026</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="38">
+        <v>33</v>
+      </c>
+      <c r="I37" s="56">
+        <v>730</v>
+      </c>
+      <c r="J37" s="38">
         <v>296</v>
       </c>
-      <c r="I37" s="33">
+      <c r="K37" s="30">
         <v>1026</v>
       </c>
-      <c r="J37" s="46">
+      <c r="L37" s="38">
         <v>296</v>
       </c>
-      <c r="K37" s="31">
-        <v>1026</v>
-      </c>
-      <c r="L37" s="46">
+      <c r="O37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P37" s="59">
+        <f t="shared" si="7"/>
+        <v>3.2163742690058478E-2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R37" s="59">
+        <f t="shared" si="9"/>
+        <v>0.40547945205479452</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T37" s="59">
+        <f t="shared" si="11"/>
+        <v>0.28849902534113059</v>
+      </c>
+      <c r="V37" s="36">
+        <v>995.2</v>
+      </c>
+      <c r="W37">
+        <v>30.15757575757576</v>
+      </c>
+    </row>
+    <row r="38" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F38" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="36">
+        <v>1039</v>
+      </c>
+      <c r="H38" s="39">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F38" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="44">
+      <c r="I38" s="57">
+        <v>733</v>
+      </c>
+      <c r="J38" s="39">
+        <v>306</v>
+      </c>
+      <c r="K38" s="36">
         <v>1039</v>
       </c>
-      <c r="H38" s="47">
+      <c r="L38" s="39">
         <v>306</v>
       </c>
-      <c r="I38" s="45">
-        <v>1039</v>
-      </c>
-      <c r="J38" s="47">
-        <v>306</v>
-      </c>
-      <c r="K38" s="44">
-        <v>1039</v>
-      </c>
-      <c r="L38" s="47">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P38" s="59">
+        <f t="shared" si="7"/>
+        <v>3.1761308950914342E-2</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R38" s="59">
+        <f t="shared" si="9"/>
+        <v>0.417462482946794</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T38" s="59">
+        <f t="shared" si="11"/>
+        <v>0.29451395572666028</v>
+      </c>
+      <c r="V38" s="30">
+        <v>4250</v>
+      </c>
+      <c r="W38">
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F39" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="G39" s="31">
+      <c r="G39" s="30">
         <v>1006</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="38">
+        <v>33</v>
+      </c>
+      <c r="I39" s="56">
+        <v>706.4</v>
+      </c>
+      <c r="J39" s="38">
         <v>299.60000000000002</v>
       </c>
-      <c r="I39" s="33">
+      <c r="K39" s="30">
         <v>1006</v>
       </c>
-      <c r="J39" s="46">
+      <c r="L39" s="38">
         <v>299.60000000000002</v>
       </c>
-      <c r="K39" s="31">
+      <c r="O39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P39" s="59">
+        <f t="shared" si="7"/>
+        <v>3.2803180914512925E-2</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R39" s="59">
+        <f t="shared" si="9"/>
+        <v>0.4241223103057758</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T39" s="59">
+        <f t="shared" si="11"/>
+        <v>0.29781312127236581</v>
+      </c>
+      <c r="V39" s="30">
+        <v>5750</v>
+      </c>
+      <c r="W39">
+        <v>11.23046875</v>
+      </c>
+    </row>
+    <row r="40" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F40" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="36">
         <v>1006</v>
       </c>
-      <c r="L39" s="46">
+      <c r="H40" s="39">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F40" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="G40" s="44">
+      <c r="I40" s="57">
+        <v>703</v>
+      </c>
+      <c r="J40" s="39">
+        <v>303</v>
+      </c>
+      <c r="K40" s="36">
         <v>1006</v>
       </c>
-      <c r="H40" s="47">
+      <c r="L40" s="39">
         <v>303</v>
       </c>
-      <c r="I40" s="45">
-        <v>1006</v>
-      </c>
-      <c r="J40" s="47">
-        <v>303</v>
-      </c>
-      <c r="K40" s="44">
-        <v>1006</v>
-      </c>
-      <c r="L40" s="47">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P40" s="59">
+        <f t="shared" si="7"/>
+        <v>3.2803180914512925E-2</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R40" s="59">
+        <f t="shared" si="9"/>
+        <v>0.43100995732574682</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T40" s="59">
+        <f t="shared" si="11"/>
+        <v>0.30119284294234594</v>
+      </c>
+      <c r="V40" s="30">
+        <v>3780</v>
+      </c>
+      <c r="W40">
+        <v>8.6896551724137936</v>
+      </c>
+    </row>
+    <row r="41" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F41" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="31">
+      <c r="G41" s="30">
         <v>585</v>
       </c>
-      <c r="H41" s="46">
+      <c r="H41" s="38"/>
+      <c r="I41" s="56">
+        <v>435</v>
+      </c>
+      <c r="J41" s="38">
         <v>150</v>
       </c>
-      <c r="I41" s="33">
+      <c r="K41" s="30">
         <v>585</v>
       </c>
-      <c r="J41" s="46">
+      <c r="L41" s="38">
         <v>150</v>
       </c>
-      <c r="K41" s="31">
-        <v>585</v>
-      </c>
-      <c r="L41" s="46"/>
-    </row>
-    <row r="42" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F42" s="43" t="s">
+      <c r="P41" s="59"/>
+      <c r="Q41">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="59">
+        <f t="shared" si="9"/>
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T41" s="59">
+        <f t="shared" si="11"/>
+        <v>0.25641025641025644</v>
+      </c>
+      <c r="V41" s="36">
+        <v>3640</v>
+      </c>
+      <c r="W41">
+        <v>8.3678160919540225</v>
+      </c>
+    </row>
+    <row r="42" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F42" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="44">
+      <c r="G42" s="36">
         <v>1471</v>
       </c>
-      <c r="H42" s="47">
+      <c r="H42" s="39"/>
+      <c r="I42" s="57">
+        <v>845</v>
+      </c>
+      <c r="J42" s="39">
         <v>626</v>
       </c>
-      <c r="I42" s="45">
+      <c r="K42" s="36">
         <v>1471</v>
       </c>
-      <c r="J42" s="47">
+      <c r="L42" s="39">
         <v>626</v>
       </c>
-      <c r="K42" s="44">
-        <v>1471</v>
-      </c>
-      <c r="L42" s="47"/>
-    </row>
-    <row r="43" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="P42" s="59"/>
+      <c r="Q42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R42" s="59">
+        <f t="shared" si="9"/>
+        <v>0.74082840236686387</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T42" s="59">
+        <f t="shared" si="11"/>
+        <v>0.42556084296397007</v>
+      </c>
+      <c r="V42" s="36">
+        <v>5700</v>
+      </c>
+      <c r="W42">
+        <v>7.5396825396825395</v>
+      </c>
+    </row>
+    <row r="43" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F43" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G43" s="31">
+      <c r="G43" s="30">
         <v>93037</v>
       </c>
-      <c r="H43" s="46">
+      <c r="H43" s="38">
+        <v>37628</v>
+      </c>
+      <c r="I43" s="56">
+        <v>44151</v>
+      </c>
+      <c r="J43" s="38">
+        <v>48826</v>
+      </c>
+      <c r="K43" s="30">
+        <v>93032</v>
+      </c>
+      <c r="L43" s="38">
+        <v>48826</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P43" s="59">
+        <f t="shared" si="7"/>
+        <v>0.40444124380622765</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R43" s="59">
+        <f>J43/I43</f>
+        <v>1.1058866163846799</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T43" s="59">
+        <f t="shared" si="11"/>
+        <v>0.52483016596439935</v>
+      </c>
+      <c r="V43" s="30">
+        <v>49972</v>
+      </c>
+      <c r="W43">
+        <v>2.2788088832140088</v>
+      </c>
+    </row>
+    <row r="44" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="36">
+        <v>60075</v>
+      </c>
+      <c r="H44" s="39">
+        <v>25000</v>
+      </c>
+      <c r="I44" s="57">
+        <v>25252</v>
+      </c>
+      <c r="J44" s="39">
+        <v>34823</v>
+      </c>
+      <c r="K44" s="36">
+        <v>60075</v>
+      </c>
+      <c r="L44" s="39">
+        <v>34823</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P44" s="59">
+        <f t="shared" si="7"/>
+        <v>0.4161464835622139</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R44" s="59">
+        <f>J44/I44</f>
+        <v>1.3790194836052589</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T44" s="59">
+        <f t="shared" si="11"/>
+        <v>0.57965875988347892</v>
+      </c>
+      <c r="V44" s="31">
+        <v>93037</v>
+      </c>
+      <c r="W44">
+        <v>1.9031420038456819</v>
+      </c>
+    </row>
+    <row r="45" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F45" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="30">
+        <v>45001</v>
+      </c>
+      <c r="H45" s="38">
+        <v>6532</v>
+      </c>
+      <c r="I45" s="60">
+        <v>28043</v>
+      </c>
+      <c r="J45" s="38">
+        <v>16958</v>
+      </c>
+      <c r="K45" s="30">
+        <v>49972</v>
+      </c>
+      <c r="L45" s="38">
+        <v>19576</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P45" s="59">
+        <f>H45/G45</f>
+        <v>0.14515232994822339</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="59">
+        <f t="shared" si="9"/>
+        <v>0.60471418892415219</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="T45" s="59">
+        <f t="shared" ref="T45" si="12">L45/K45</f>
+        <v>0.39173937404946768</v>
+      </c>
+    </row>
+    <row r="46" spans="6:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" s="63">
+        <v>28819</v>
+      </c>
+      <c r="H46" s="61">
+        <v>6532</v>
+      </c>
+      <c r="I46" s="62">
+        <v>19152</v>
+      </c>
+      <c r="J46" s="64">
+        <v>9667</v>
+      </c>
+      <c r="K46" s="62">
+        <v>28819</v>
+      </c>
+      <c r="L46" s="64">
+        <v>9667</v>
+      </c>
+      <c r="M46" s="31"/>
+      <c r="N46" s="33"/>
+      <c r="O46" s="33">
+        <f t="shared" ref="O46" si="13">G46/G46</f>
+        <v>1</v>
+      </c>
+      <c r="P46" s="65">
+        <f>H46/G46</f>
+        <v>0.22665602553870709</v>
+      </c>
+      <c r="Q46" s="33">
+        <f t="shared" ref="Q46" si="14">I46/I46</f>
+        <v>1</v>
+      </c>
+      <c r="R46" s="65">
+        <f t="shared" ref="R46" si="15">J46/I46</f>
+        <v>0.50475146198830412</v>
+      </c>
+      <c r="S46" s="33">
+        <f t="shared" ref="S46" si="16">K46/K46</f>
+        <v>1</v>
+      </c>
+      <c r="T46" s="65">
+        <f t="shared" ref="T46" si="17">L46/K46</f>
+        <v>0.33543842603837748</v>
+      </c>
+    </row>
+    <row r="47" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="P47" s="59">
+        <f>AVERAGE(P31:P45)</f>
+        <v>0.12732913745084748</v>
+      </c>
+      <c r="R47" s="59">
+        <f>AVERAGE(R31:R46)</f>
+        <v>0.58217148665197416</v>
+      </c>
+      <c r="T47" s="59">
+        <f>AVERAGE(T31:T45)</f>
+        <v>0.35336705833018628</v>
+      </c>
+    </row>
+    <row r="48" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="R48" s="59">
+        <f>AVERAGE(R31:R42)</f>
+        <v>0.4766976696274326</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F52" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52" s="8">
+        <v>93037</v>
+      </c>
+      <c r="H52" s="9">
         <v>48886</v>
       </c>
-      <c r="I43" s="33">
-        <v>93037</v>
-      </c>
-      <c r="J43" s="46">
-        <v>48886</v>
-      </c>
-      <c r="K43" s="31">
-        <v>93037</v>
-      </c>
-      <c r="L43" s="46">
-        <v>48886</v>
-      </c>
-    </row>
-    <row r="44" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F44" s="43" t="s">
+      <c r="I52" s="10">
+        <v>37628</v>
+      </c>
+      <c r="J52" s="10">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F53" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G53" s="8">
         <v>60075</v>
       </c>
-      <c r="H44" s="47">
+      <c r="H53" s="9">
         <v>34823</v>
       </c>
-      <c r="I44" s="45">
-        <v>60075</v>
-      </c>
-      <c r="J44" s="47">
-        <v>34823</v>
-      </c>
-      <c r="K44" s="44">
-        <v>60075</v>
-      </c>
-      <c r="L44" s="47">
-        <v>34823</v>
-      </c>
-    </row>
-    <row r="45" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="35" t="s">
+      <c r="I53" s="10">
+        <v>25000</v>
+      </c>
+      <c r="J53" s="10">
+        <v>25252</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F54" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="G45" s="32">
-        <v>49972</v>
-      </c>
-      <c r="H45" s="48">
-        <v>19576</v>
-      </c>
-      <c r="I45" s="34">
-        <v>49972</v>
-      </c>
-      <c r="J45" s="48">
-        <v>19576</v>
-      </c>
-      <c r="K45" s="32">
-        <v>49972</v>
-      </c>
-      <c r="L45" s="48">
-        <v>21929</v>
+      <c r="G54" s="8">
+        <v>45001</v>
+      </c>
+      <c r="H54" s="8">
+        <v>16958</v>
+      </c>
+      <c r="I54" s="8">
+        <v>6532</v>
+      </c>
+      <c r="J54" s="8">
+        <v>28043</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G55" s="18">
+        <v>28819</v>
+      </c>
+      <c r="H55" s="18">
+        <v>9667</v>
+      </c>
+      <c r="I55" s="8">
+        <v>6532</v>
+      </c>
+      <c r="J55" s="8">
+        <v>19152</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="V33:W44">
+    <sortCondition descending="1" ref="W33:W44"/>
+  </sortState>
+  <mergeCells count="17">
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="F12:L12"/>
@@ -4158,496 +6827,336 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80C5C0-5165-4D8F-8D34-D728F416EF6B}">
-  <dimension ref="A1:N16"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD847D4-F568-4E09-8F78-4359FC462EB7}">
+  <dimension ref="B2:V7"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="H3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>5750</v>
-      </c>
-      <c r="C2">
-        <v>1880</v>
-      </c>
-      <c r="D2">
-        <v>512</v>
-      </c>
-      <c r="E2">
-        <v>3350</v>
-      </c>
-      <c r="F2">
-        <v>1880</v>
-      </c>
-      <c r="G2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H2">
-        <v>9.9000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3">
-        <v>5700</v>
-      </c>
-      <c r="C3">
-        <v>1814</v>
-      </c>
-      <c r="D3">
-        <v>756</v>
-      </c>
-      <c r="E3">
-        <v>3820</v>
-      </c>
-      <c r="F3">
-        <v>1058</v>
-      </c>
-      <c r="G3">
-        <v>0.67</v>
-      </c>
-      <c r="H3">
-        <v>0.153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4">
-        <v>3780</v>
-      </c>
-      <c r="C4">
-        <v>1200</v>
-      </c>
-      <c r="D4" s="29">
-        <v>435</v>
-      </c>
-      <c r="E4">
-        <v>2580</v>
-      </c>
-      <c r="F4">
-        <v>765</v>
-      </c>
-      <c r="G4">
-        <v>0.68</v>
-      </c>
-      <c r="H4">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5">
-        <v>3640</v>
-      </c>
-      <c r="C5">
-        <v>1200</v>
-      </c>
-      <c r="D5" s="29">
-        <v>435</v>
-      </c>
-      <c r="E5">
-        <v>2440</v>
-      </c>
-      <c r="F5">
-        <v>765</v>
-      </c>
-      <c r="G5">
-        <v>0.67</v>
-      </c>
-      <c r="H5">
-        <v>0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6">
-        <v>4250</v>
-      </c>
-      <c r="C6">
-        <v>1497</v>
-      </c>
-      <c r="D6">
-        <v>300</v>
-      </c>
-      <c r="E6">
-        <v>2753</v>
-      </c>
-      <c r="F6">
-        <v>1197</v>
-      </c>
-      <c r="G6">
-        <v>0.65</v>
-      </c>
-      <c r="H6">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="J6">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7">
-        <v>995.2</v>
-      </c>
-      <c r="C7">
-        <v>294.3</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <v>700.9</v>
-      </c>
-      <c r="G7">
-        <v>0.7</v>
-      </c>
-      <c r="H7">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8">
-        <v>1026</v>
-      </c>
-      <c r="C8">
-        <v>296</v>
-      </c>
-      <c r="D8">
-        <v>33</v>
-      </c>
-      <c r="E8">
-        <v>730</v>
-      </c>
-      <c r="G8">
-        <v>0.71</v>
-      </c>
-      <c r="H8">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9">
-        <v>1039</v>
-      </c>
-      <c r="C9">
-        <v>306</v>
-      </c>
-      <c r="D9">
-        <v>33</v>
-      </c>
-      <c r="E9">
-        <v>733</v>
-      </c>
-      <c r="G9">
-        <v>0.71</v>
-      </c>
-      <c r="H9">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10">
-        <v>1006</v>
-      </c>
-      <c r="C10">
-        <v>299.60000000000002</v>
-      </c>
-      <c r="D10">
-        <v>33</v>
-      </c>
-      <c r="E10">
-        <v>706.4</v>
-      </c>
-      <c r="G10">
-        <v>0.7</v>
-      </c>
-      <c r="H10">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11">
-        <v>1006</v>
-      </c>
-      <c r="C11">
-        <v>303</v>
-      </c>
-      <c r="D11">
-        <v>33</v>
-      </c>
-      <c r="E11">
-        <v>703</v>
-      </c>
-      <c r="G11">
-        <v>0.7</v>
-      </c>
-      <c r="H11">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12">
-        <v>585</v>
-      </c>
-      <c r="C12">
-        <v>150</v>
-      </c>
-      <c r="E12">
-        <v>435</v>
-      </c>
-      <c r="G12">
-        <v>0.74</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13">
-        <v>1471</v>
-      </c>
-      <c r="C13">
-        <v>626</v>
-      </c>
-      <c r="E13">
-        <v>845</v>
-      </c>
-      <c r="G13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="8">
-        <v>93037</v>
-      </c>
-      <c r="C14" s="9">
-        <v>48886</v>
-      </c>
-      <c r="D14" s="10">
-        <v>48886</v>
-      </c>
-      <c r="E14" s="10">
-        <v>35894</v>
-      </c>
-      <c r="F14" s="10">
-        <v>44151</v>
-      </c>
-      <c r="G14" s="11">
-        <v>11198</v>
-      </c>
-      <c r="H14" s="10">
-        <v>307</v>
-      </c>
-      <c r="I14" s="10">
-        <v>385</v>
-      </c>
-      <c r="J14" s="10">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
-        <v>1770</v>
-      </c>
-      <c r="L14" s="11">
-        <v>4969</v>
-      </c>
-      <c r="M14" s="8">
+      <c r="N3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8">
+        <v>15103</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4479</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6855</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4821</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10624</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2034</v>
+      </c>
+      <c r="I4" s="66">
+        <v>192.8394236030887</v>
+      </c>
+      <c r="J4" s="66">
+        <v>641.8797957074238</v>
+      </c>
+      <c r="K4" s="66">
+        <v>461.8963336778744</v>
+      </c>
+      <c r="L4" s="66">
+        <v>1064</v>
+      </c>
+      <c r="M4" s="66">
+        <v>517</v>
+      </c>
+      <c r="N4" s="8">
+        <v>80068</v>
+      </c>
+      <c r="O4" s="8">
+        <v>23130.9</v>
+      </c>
+      <c r="P4" s="8">
+        <v>10282</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>2034</v>
+      </c>
+      <c r="R4" s="8">
+        <v>4821</v>
+      </c>
+      <c r="S4" s="8">
+        <v>2445</v>
+      </c>
+      <c r="T4" s="8">
+        <v>8248</v>
+      </c>
+      <c r="U4" s="8">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="8">
+        <v>16447</v>
+      </c>
+      <c r="D5" s="9">
+        <v>5113</v>
+      </c>
+      <c r="E5" s="10">
+        <v>7667</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4795</v>
+      </c>
+      <c r="G5" s="10">
+        <v>11019</v>
+      </c>
+      <c r="H5" s="11">
+        <v>2872</v>
+      </c>
+      <c r="I5" s="10">
+        <v>210</v>
+      </c>
+      <c r="J5" s="10">
+        <v>699</v>
+      </c>
+      <c r="K5" s="10">
+        <v>503</v>
+      </c>
+      <c r="L5" s="10">
+        <v>925</v>
+      </c>
+      <c r="M5" s="11">
+        <v>818</v>
+      </c>
+      <c r="N5" s="8">
+        <v>80068</v>
+      </c>
+      <c r="O5" s="8">
+        <v>23130.9</v>
+      </c>
+      <c r="P5" s="8">
+        <v>11652</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>2872</v>
+      </c>
+      <c r="R5" s="8">
+        <v>4795</v>
+      </c>
+      <c r="S5" s="8">
+        <v>2241</v>
+      </c>
+      <c r="T5" s="8">
+        <v>8527</v>
+      </c>
+      <c r="U5" s="8">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="8">
+        <v>45862</v>
+      </c>
+      <c r="D6" s="17">
+        <v>15425</v>
+      </c>
+      <c r="E6" s="18">
+        <v>20271</v>
+      </c>
+      <c r="F6" s="18">
+        <v>14135</v>
+      </c>
+      <c r="G6" s="18">
+        <v>29820</v>
+      </c>
+      <c r="H6" s="16">
+        <v>11264</v>
+      </c>
+      <c r="I6" s="18">
+        <v>454</v>
+      </c>
+      <c r="J6" s="18">
+        <v>468</v>
+      </c>
+      <c r="K6" s="18">
+        <v>1177</v>
+      </c>
+      <c r="L6" s="18">
+        <v>2138</v>
+      </c>
+      <c r="M6" s="16">
+        <v>3255</v>
+      </c>
+      <c r="N6" s="18">
         <v>266800</v>
       </c>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="8">
-        <v>60075</v>
-      </c>
-      <c r="C15" s="9">
-        <v>34823</v>
-      </c>
-      <c r="D15" s="10">
-        <v>34823</v>
-      </c>
-      <c r="E15" s="10">
-        <v>25000</v>
-      </c>
-      <c r="F15" s="10">
-        <v>25252</v>
-      </c>
-      <c r="G15" s="11">
-        <v>9823</v>
-      </c>
-      <c r="H15" s="10">
-        <v>898</v>
-      </c>
-      <c r="I15" s="10">
-        <v>478</v>
-      </c>
-      <c r="J15" s="10">
-        <v>2017</v>
-      </c>
-      <c r="K15" s="10">
-        <v>1681</v>
-      </c>
-      <c r="L15" s="11">
-        <v>822</v>
-      </c>
-      <c r="M15" s="8">
-        <v>177929</v>
-      </c>
-      <c r="N15" s="8">
-        <v>177929</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="8">
-        <v>49972</v>
-      </c>
-      <c r="C16" s="8">
-        <v>19576</v>
-      </c>
-      <c r="D16" s="8">
-        <v>21929</v>
-      </c>
-      <c r="E16" s="8">
-        <v>14234</v>
-      </c>
-      <c r="F16" s="8">
-        <v>30396</v>
-      </c>
-      <c r="G16" s="8">
-        <v>9672</v>
-      </c>
-      <c r="H16" s="8">
-        <v>693</v>
-      </c>
-      <c r="I16" s="8">
-        <v>1288</v>
-      </c>
-      <c r="J16" s="8">
-        <v>312</v>
-      </c>
-      <c r="K16" s="8">
-        <v>1905</v>
-      </c>
-      <c r="L16" s="8">
-        <v>3036</v>
-      </c>
-      <c r="M16" s="8">
-        <v>44482.2</v>
-      </c>
-      <c r="N16" s="8">
-        <v>15568</v>
+      <c r="O6" s="18">
+        <v>44500</v>
+      </c>
+      <c r="P6" s="18">
+        <v>35054</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>9463</v>
+      </c>
+      <c r="R6" s="18">
+        <v>10808</v>
+      </c>
+      <c r="S6" s="18">
+        <v>5962</v>
+      </c>
+      <c r="T6" s="18">
+        <v>25105</v>
+      </c>
+      <c r="U6" s="18">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="8">
+        <v>81911</v>
+      </c>
+      <c r="D7" s="17">
+        <v>26912</v>
+      </c>
+      <c r="E7" s="18">
+        <v>51994</v>
+      </c>
+      <c r="F7" s="18">
+        <v>10790</v>
+      </c>
+      <c r="G7" s="18">
+        <v>54360</v>
+      </c>
+      <c r="H7" s="16">
+        <v>23813</v>
+      </c>
+      <c r="I7" s="18">
+        <v>875</v>
+      </c>
+      <c r="J7" s="18">
+        <v>1299</v>
+      </c>
+      <c r="K7" s="18">
+        <v>2189</v>
+      </c>
+      <c r="L7" s="18">
+        <v>6452</v>
+      </c>
+      <c r="M7" s="16">
+        <v>4840</v>
+      </c>
+      <c r="N7" s="18">
+        <v>200100</v>
+      </c>
+      <c r="O7" s="18">
+        <v>140192</v>
+      </c>
+      <c r="P7" s="18">
+        <v>39791</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>9874</v>
+      </c>
+      <c r="R7" s="18">
+        <v>31330</v>
+      </c>
+      <c r="S7" s="18">
+        <v>6618</v>
+      </c>
+      <c r="T7" s="18">
+        <v>29769</v>
+      </c>
+      <c r="U7" s="18">
+        <v>24508</v>
       </c>
     </row>
   </sheetData>
@@ -4656,7 +7165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77947650-EFE6-4BC5-8EC3-7F1726132A86}">
   <dimension ref="A1:U4"/>
   <sheetViews>

</xml_diff>